<commit_message>
Updated the scrum spreadsheet to match finished work
</commit_message>
<xml_diff>
--- a/P10/Scrum_Sprint_4.xlsx
+++ b/P10/Scrum_Sprint_4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Desktop\cse1325\P10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306F3BBA-1717-498B-8EF6-7AD03FBDC42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA1B3C1-D8DA-49AB-94BD-64A0D9B77B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39345" yWindow="1620" windowWidth="12690" windowHeight="7695" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="167">
   <si>
     <t>Product Name:</t>
   </si>
@@ -515,7 +515,34 @@
     <t>NOTE: This sprint is entirely OPTIONAL – no points will be lost if you ignore it</t>
   </si>
   <si>
-    <t>Not Started</t>
+    <t>Finished in Sprint 1</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 2</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 3</t>
+  </si>
+  <si>
+    <t>Finished in Spring 3</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 4</t>
+  </si>
+  <si>
+    <t>Insert orders through gue</t>
+  </si>
+  <si>
+    <t>Calculate the cost of each order</t>
+  </si>
+  <si>
+    <t>List orders in main window</t>
+  </si>
+  <si>
+    <t>Rid this world of horrid multy step dialogs</t>
+  </si>
+  <si>
+    <t>Completed Day 2</t>
   </si>
 </sst>
 </file>
@@ -1029,19 +1056,19 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1248,7 +1275,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -1397,7 +1424,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -1471,7 +1498,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -1562,7 +1589,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -1711,7 +1738,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -1785,7 +1812,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -1876,7 +1903,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -2025,7 +2052,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -2099,7 +2126,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -2190,7 +2217,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -2268,28 +2295,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2339,7 +2366,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -2413,7 +2440,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -3702,8 +3729,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -3903,11 +3930,11 @@
       </c>
       <c r="B13" s="5">
         <f>B12-C13</f>
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C13" s="9">
         <f>COUNTIF(G$24:G$107,"Finished in Sprint 1")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="5"/>
@@ -3927,11 +3954,11 @@
       </c>
       <c r="B14" s="5">
         <f>B13-C14</f>
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C14" s="9">
         <f>COUNTIF(G$24:G$107,"Finished in Sprint 2")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="5"/>
@@ -3951,11 +3978,11 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$107,"Finished in Sprint 3")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="5"/>
@@ -3975,11 +4002,11 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$107,"Finished in Sprint 4")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="5"/>
@@ -3995,11 +4022,11 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$107,"Finished in Sprint 4")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="5"/>
@@ -4126,8 +4153,12 @@
       <c r="E24" s="16">
         <v>3</v>
       </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
+      <c r="F24" s="17">
+        <v>1</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>157</v>
+      </c>
       <c r="H24" s="18" t="s">
         <v>31</v>
       </c>
@@ -4155,8 +4186,12 @@
       <c r="E25" s="16">
         <v>3</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
+      <c r="F25" s="17">
+        <v>1</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>157</v>
+      </c>
       <c r="H25" s="18" t="s">
         <v>36</v>
       </c>
@@ -4184,8 +4219,12 @@
       <c r="E26" s="16">
         <v>8</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="F26" s="17">
+        <v>1</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>157</v>
+      </c>
       <c r="H26" s="18" t="s">
         <v>31</v>
       </c>
@@ -4211,8 +4250,12 @@
       <c r="E27" s="16">
         <v>8</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
+      <c r="F27" s="17">
+        <v>1</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>157</v>
+      </c>
       <c r="H27" s="18" t="s">
         <v>31</v>
       </c>
@@ -4238,8 +4281,12 @@
       <c r="E28" s="16">
         <v>13</v>
       </c>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
+      <c r="F28" s="17">
+        <v>1</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>157</v>
+      </c>
       <c r="H28" s="18" t="s">
         <v>31</v>
       </c>
@@ -4265,8 +4312,12 @@
       <c r="E29" s="21">
         <v>13</v>
       </c>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
+      <c r="F29" s="17">
+        <v>2</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>158</v>
+      </c>
       <c r="H29" s="18" t="s">
         <v>31</v>
       </c>
@@ -4294,8 +4345,12 @@
       <c r="E30" s="21">
         <v>5</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
+      <c r="F30" s="17">
+        <v>2</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>158</v>
+      </c>
       <c r="H30" s="18" t="s">
         <v>31</v>
       </c>
@@ -4323,8 +4378,12 @@
       <c r="E31" s="21">
         <v>3</v>
       </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
+      <c r="F31" s="17">
+        <v>2</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>158</v>
+      </c>
       <c r="H31" s="18" t="s">
         <v>31</v>
       </c>
@@ -4350,8 +4409,12 @@
       <c r="E32" s="21">
         <v>5</v>
       </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
+      <c r="F32" s="17">
+        <v>2</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>159</v>
+      </c>
       <c r="H32" s="18" t="s">
         <v>31</v>
       </c>
@@ -4377,8 +4440,12 @@
       <c r="E33" s="21">
         <v>5</v>
       </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
+      <c r="F33" s="17">
+        <v>2</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>158</v>
+      </c>
       <c r="H33" s="18" t="s">
         <v>31</v>
       </c>
@@ -4406,8 +4473,12 @@
       <c r="E34" s="21">
         <v>8</v>
       </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
+      <c r="F34" s="17">
+        <v>2</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>158</v>
+      </c>
       <c r="H34" s="18" t="s">
         <v>31</v>
       </c>
@@ -4435,8 +4506,12 @@
       <c r="E35" s="42">
         <v>2</v>
       </c>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
+      <c r="F35" s="17">
+        <v>2</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>158</v>
+      </c>
       <c r="H35" s="18" t="s">
         <v>70</v>
       </c>
@@ -4464,8 +4539,12 @@
       <c r="E36" s="16">
         <v>5</v>
       </c>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
+      <c r="F36" s="17">
+        <v>3</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>159</v>
+      </c>
       <c r="H36" s="18" t="s">
         <v>70</v>
       </c>
@@ -4493,8 +4572,12 @@
       <c r="E37" s="16">
         <v>13</v>
       </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
+      <c r="F37" s="17">
+        <v>3</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>159</v>
+      </c>
       <c r="H37" s="18" t="s">
         <v>79</v>
       </c>
@@ -4522,8 +4605,12 @@
       <c r="E38" s="16">
         <v>1</v>
       </c>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
+      <c r="F38" s="17">
+        <v>3</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>159</v>
+      </c>
       <c r="H38" s="18" t="s">
         <v>79</v>
       </c>
@@ -4551,8 +4638,12 @@
       <c r="E39" s="16">
         <v>5</v>
       </c>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
+      <c r="F39" s="17">
+        <v>3</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>159</v>
+      </c>
       <c r="H39" s="18" t="s">
         <v>79</v>
       </c>
@@ -4580,8 +4671,12 @@
       <c r="E40" s="16">
         <v>8</v>
       </c>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
+      <c r="F40" s="17">
+        <v>3</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>160</v>
+      </c>
       <c r="H40" s="18" t="s">
         <v>79</v>
       </c>
@@ -4613,7 +4708,7 @@
         <v>4</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H41" s="18" t="s">
         <v>31</v>
@@ -4644,7 +4739,7 @@
         <v>4</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H42" s="18" t="s">
         <v>31</v>
@@ -4675,7 +4770,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H43" s="18" t="s">
         <v>31</v>
@@ -4708,7 +4803,7 @@
         <v>4</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H44" s="18" t="s">
         <v>31</v>
@@ -5626,7 +5721,7 @@
       <formula1>"1,2,3,4"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank initially (hint: Use the Delete key)_x000a_Select &quot;In Work&quot; when you begin designing and coding this feature._x000a_Select &quot;In Test&quot; when this feature is fully coded and you are testing it._x000a_Select  Finished ONLY when the feature works well and is READY TO" sqref="G24:G101" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank initially (hint: Use the Delete key)_x000a_Select &quot;In Work&quot; when you begin designing and coding this feature._x000a_Select &quot;In Test&quot; when this feature is fully coded and you are testing it._x000a_Select  Finished ONLY when the feature works well and is READY TO" sqref="G41:G101 G24:G39" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>"Not Started,In Work,In Test,Finished in Sprint 1,Finished in Sprint 2,Finished in Sprint 3,Finished in Sprint 4,Finished in Sprint 5,Finished in Sprint 6"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9153,8 +9248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -9258,7 +9353,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -9273,7 +9368,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -9291,11 +9386,11 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -9309,7 +9404,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -9327,7 +9422,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -9345,7 +9440,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -9363,7 +9458,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -9381,7 +9476,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -9427,42 +9522,64 @@
       <c r="A17" s="4">
         <v>1</v>
       </c>
-      <c r="B17" s="35"/>
+      <c r="B17" s="35" t="s">
+        <v>92</v>
+      </c>
       <c r="C17" s="4"/>
       <c r="D17" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="E17" s="37"/>
+        <v>162</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>166</v>
+      </c>
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B18" s="35"/>
+      <c r="B18" s="35" t="s">
+        <v>94</v>
+      </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="37"/>
+      <c r="D18" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>166</v>
+      </c>
       <c r="F18" s="38"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>3</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="35" t="s">
+        <v>97</v>
+      </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="37"/>
+      <c r="D19" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>166</v>
+      </c>
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B20" s="35"/>
+      <c r="B20" s="35" t="s">
+        <v>101</v>
+      </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="37"/>
+      <c r="D20" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>166</v>
+      </c>
       <c r="F20" s="38"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>